<commit_message>
Se agregaron documentos del Sprint 1
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Requisitos/Product Backlog.xlsx
+++ b/Desarrollo/Edutec/Requisitos/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C483E15-95FF-460F-B4AF-2508C90F7B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9D7540-A1C0-41D0-ABC7-580DF1533756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="12" r:id="rId1"/>
@@ -26,8 +26,17 @@
     <sheet name="CA_D_INSITUTOS" sheetId="10" r:id="rId11"/>
     <sheet name="CA_REPORTES" sheetId="11" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId15" roundtripDataSignature="AMtx7miFo66tI5Krd8N3QFh+myzfHXGpsw=="/>
     </ext>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Modificación de Historias de Usuario</t>
   </si>
@@ -301,6 +310,18 @@
   <si>
     <t>Product Backlog</t>
   </si>
+  <si>
+    <t>T02</t>
+  </si>
+  <si>
+    <t>Recuperar contraseña</t>
+  </si>
+  <si>
+    <t>deseo restablecer mi contraseña</t>
+  </si>
+  <si>
+    <t>para poder ingresar al sistema en caso haya olvidado mi contraseña</t>
+  </si>
 </sst>
 </file>
 
@@ -483,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -542,6 +563,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,9 +1009,9 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2838450" cy="1371600"/>
+    <xdr:ext cx="2838450" cy="1895475"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Shape 6">
@@ -995,8 +1025,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12430125" y="4191000"/>
-          <a:ext cx="2838450" cy="1371600"/>
+          <a:off x="12430125" y="4190999"/>
+          <a:ext cx="2838450" cy="1895475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1039,8 +1069,72 @@
               <a:cs typeface="Calibri"/>
               <a:sym typeface="Calibri"/>
             </a:rPr>
-            <a:t>Debe admitir caracteres alfanúmericos y no debe tener ninguna restricción de validación de mayusculas, caracteres especiales, etc.</a:t>
+            <a:t>Debe admitir caracteres alfanúmericos y no debe tener ninguna restricción de validación de mayusculas, caracteres especiales, etc. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" rtl="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+              <a:sym typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Longitud</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+              <a:sym typeface="Calibri"/>
+            </a:rPr>
+            <a:t> mínima de 8 caracteres.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" lvl="0" indent="0" algn="l" rtl="0">
@@ -1312,9 +1406,9 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>28572</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2571751" cy="1038243"/>
+    <xdr:ext cx="2571751" cy="1300173"/>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="10" name="Shape 2">
@@ -1328,10 +1422,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9858374" y="3838575"/>
-          <a:ext cx="2571751" cy="1038243"/>
+          <a:off x="9858374" y="3838572"/>
+          <a:ext cx="2571751" cy="1300173"/>
           <a:chOff x="4041075" y="4317263"/>
-          <a:chExt cx="2600071" cy="87969"/>
+          <a:chExt cx="2600071" cy="110162"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -1350,7 +1444,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="4041075" y="4317263"/>
-            <a:ext cx="2600071" cy="87969"/>
+            <a:ext cx="2600071" cy="110162"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -9142,10 +9236,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9410,7 +9504,7 @@
       <c r="Z8" s="12"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -9420,7 +9514,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>69</v>
@@ -9454,7 +9548,7 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="8" t="s">
         <v>67</v>
       </c>
@@ -9496,29 +9590,27 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>61</v>
-      </c>
+      <c r="A11" s="30"/>
       <c r="B11" s="8" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="G11" s="7">
         <v>85</v>
       </c>
       <c r="H11" s="6">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -9540,27 +9632,29 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="B12" s="8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G12" s="7">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H12" s="6">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -9582,29 +9676,27 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="A13" s="26"/>
       <c r="B13" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G13" s="7">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H13" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -9626,27 +9718,29 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G14" s="7">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H14" s="6">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -9668,29 +9762,27 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>45</v>
-      </c>
+      <c r="A15" s="26"/>
       <c r="B15" s="8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G15" s="7">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H15" s="6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -9711,28 +9803,30 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="B16" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>36</v>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="G16" s="7">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H16" s="6">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -9753,27 +9847,25 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>35</v>
-      </c>
+    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
       <c r="B17" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>31</v>
+      <c r="F17" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="G17" s="7">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H17" s="6">
         <v>8</v>
@@ -9798,27 +9890,29 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="25" t="s">
+        <v>35</v>
+      </c>
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G18" s="7">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H18" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -9842,19 +9936,19 @@
     <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G19" s="7">
         <v>48</v>
@@ -9882,27 +9976,27 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="8" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G20" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H20" s="6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -9924,26 +10018,24 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="26"/>
       <c r="B21" s="8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>15</v>
+      <c r="F21" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="G21" s="7">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H21" s="6">
         <v>8</v>
@@ -9968,27 +10060,29 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25" t="s">
+        <v>19</v>
+      </c>
       <c r="B22" s="8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G22" s="7">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H22" s="6">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -10009,30 +10103,28 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>10</v>
+    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>8</v>
+      <c r="C23" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>6</v>
+      <c r="E23" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>5</v>
+      <c r="F23" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="G23" s="7">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H23" s="6">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -10053,15 +10145,31 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+    <row r="24" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="7">
+        <v>25</v>
+      </c>
+      <c r="H24" s="6">
+        <v>20</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -10193,18 +10301,12 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+    <row r="29" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -10228,17 +10330,17 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>44505</v>
+      <c r="A30" s="5" t="s">
+        <v>4</v>
       </c>
-      <c r="B30" s="3">
-        <v>1.1000000000000001</v>
+      <c r="B30" s="5" t="s">
+        <v>3</v>
       </c>
-      <c r="C30" s="24" t="s">
-        <v>1</v>
+      <c r="C30" s="23" t="s">
+        <v>2</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -10263,13 +10365,13 @@
     </row>
     <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>44519</v>
+        <v>44505</v>
       </c>
       <c r="B31" s="3">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
@@ -10295,12 +10397,18 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+    <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>44519</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -37623,17 +37731,45 @@
       <c r="Y1007" s="2"/>
       <c r="Z1007" s="2"/>
     </row>
+    <row r="1008" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1008" s="2"/>
+      <c r="B1008" s="2"/>
+      <c r="C1008" s="2"/>
+      <c r="D1008" s="2"/>
+      <c r="E1008" s="2"/>
+      <c r="F1008" s="2"/>
+      <c r="G1008" s="2"/>
+      <c r="H1008" s="2"/>
+      <c r="I1008" s="2"/>
+      <c r="J1008" s="2"/>
+      <c r="K1008" s="2"/>
+      <c r="L1008" s="2"/>
+      <c r="M1008" s="2"/>
+      <c r="N1008" s="2"/>
+      <c r="O1008" s="2"/>
+      <c r="P1008" s="2"/>
+      <c r="Q1008" s="2"/>
+      <c r="R1008" s="2"/>
+      <c r="S1008" s="2"/>
+      <c r="T1008" s="2"/>
+      <c r="U1008" s="2"/>
+      <c r="V1008" s="2"/>
+      <c r="W1008" s="2"/>
+      <c r="X1008" s="2"/>
+      <c r="Y1008" s="2"/>
+      <c r="Z1008" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A9:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40640,7 +40776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A21:A1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H13" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -43640,8 +43776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A21:A1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>